<commit_message>
modify continuousFrames addition to datalist
</commit_message>
<xml_diff>
--- a/datalists/npr1_HD_g_list.xlsx
+++ b/datalists/npr1_HD_g_list.xlsx
@@ -582,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -593,7 +593,7 @@
     <col min="1" max="1" width="93.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -621,17 +621,8 @@
       <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L1">
-        <v>29140</v>
-      </c>
-      <c r="M1">
-        <v>29210</v>
-      </c>
-      <c r="N1">
-        <v>32399</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -660,7 +651,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -687,7 +678,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -714,7 +705,7 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -741,7 +732,7 @@
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -770,7 +761,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -797,7 +788,7 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -829,7 +820,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -857,7 +848,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -886,7 +877,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -916,7 +907,7 @@
       </c>
       <c r="J11" s="1"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:10">
       <c r="F14" t="s">
         <v>12</v>
       </c>

</xml_diff>